<commit_message>
updates on crosswalk to clean up NLA location issues, and edits on AGU abstract
</commit_message>
<xml_diff>
--- a/data/surge/SuRGE_design_20191206_eval_status.xlsx
+++ b/data/surge/SuRGE_design_20191206_eval_status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/SuRGE/Shared Documents/surgeDsn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="6_{90B923AC-9DC5-4BF3-8172-F11B5FFF89E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20F43C11-8E2B-45AB-A896-76864A87B5B1}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="6_{90B923AC-9DC5-4BF3-8172-F11B5FFF89E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A848CB72-B5F7-4F84-B98E-01772583A97B}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2505" windowWidth="19440" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="1190" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SuRGE_design_20191206" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6912" uniqueCount="1810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6921" uniqueCount="1817">
   <si>
     <t>siteID</t>
   </si>
@@ -5490,6 +5490,27 @@
   </si>
   <si>
     <t>NHDPlusFlowlineCOMID</t>
+  </si>
+  <si>
+    <t>NLA_NC-10018</t>
+  </si>
+  <si>
+    <t>NLA_OH-10004</t>
+  </si>
+  <si>
+    <t>NLA_OH-10022</t>
+  </si>
+  <si>
+    <t>NLA_OH-10017</t>
+  </si>
+  <si>
+    <t>NLA_OH-10012</t>
+  </si>
+  <si>
+    <t>NLA_OH-10030</t>
+  </si>
+  <si>
+    <t>NLA_OH-10019</t>
   </si>
 </sst>
 </file>
@@ -6373,53 +6394,53 @@
   <dimension ref="A1:AI372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G347" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K342" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A349" sqref="A349"/>
+      <selection pane="bottomRight" activeCell="M343" sqref="M343"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.83984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.41796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.15625" style="3" customWidth="1"/>
     <col min="4" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="6" width="13.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="59.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="24.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.41796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.41796875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="24.68359375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.68359375" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="43.5703125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.5703125" style="2" customWidth="1"/>
-    <col min="26" max="26" width="20.42578125" style="2" customWidth="1"/>
-    <col min="27" max="27" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="24.5703125" style="2" customWidth="1"/>
-    <col min="36" max="36" width="23.42578125" customWidth="1"/>
-    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="43.578125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="13.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.578125" style="2" customWidth="1"/>
+    <col min="26" max="26" width="20.41796875" style="2" customWidth="1"/>
+    <col min="27" max="27" width="29.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="18.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="24.578125" style="2" customWidth="1"/>
+    <col min="36" max="36" width="23.41796875" customWidth="1"/>
+    <col min="37" max="37" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="32.41796875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6526,7 +6547,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
@@ -6630,7 +6651,7 @@
         <v>-524209.81246461201</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
@@ -6734,7 +6755,7 @@
         <v>-294281.450343773</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -6838,7 +6859,7 @@
         <v>-522941.95774194098</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -6942,7 +6963,7 @@
         <v>-685799.49722169002</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>92</v>
       </c>
@@ -7034,7 +7055,7 @@
         <v>-723289.36932586005</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
@@ -7129,7 +7150,7 @@
         <v>-321099.97861358401</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>79</v>
       </c>
@@ -7224,7 +7245,7 @@
         <v>-646024.81080743903</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>85</v>
       </c>
@@ -7319,7 +7340,7 @@
         <v>-333679.175147245</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>105</v>
       </c>
@@ -7420,7 +7441,7 @@
         <v>-372481.46087195602</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>112</v>
       </c>
@@ -7524,7 +7545,7 @@
         <v>-1076830.28452363</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>98</v>
       </c>
@@ -7628,7 +7649,7 @@
         <v>-624752.21894294803</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>118</v>
       </c>
@@ -7726,7 +7747,7 @@
         <v>-1269905.5328431299</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>135</v>
       </c>
@@ -7827,7 +7848,7 @@
         <v>317266.839770841</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>131</v>
       </c>
@@ -7931,7 +7952,7 @@
         <v>-612610.76208755199</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>126</v>
       </c>
@@ -8035,7 +8056,7 @@
         <v>-430362.95707428001</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>142</v>
       </c>
@@ -8139,7 +8160,7 @@
         <v>147147.79634205301</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>149</v>
       </c>
@@ -8243,7 +8264,7 @@
         <v>-1103051.8098598199</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>153</v>
       </c>
@@ -8347,7 +8368,7 @@
         <v>-738530.36143332196</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>158</v>
       </c>
@@ -8442,7 +8463,7 @@
         <v>-628186.33568704699</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>163</v>
       </c>
@@ -8537,7 +8558,7 @@
         <v>59383.704366039397</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>167</v>
       </c>
@@ -8632,7 +8653,7 @@
         <v>-43819.502321893298</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
         <v>172</v>
       </c>
@@ -8727,7 +8748,7 @@
         <v>-541640.76685755001</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>177</v>
       </c>
@@ -8822,7 +8843,7 @@
         <v>-337121.356418802</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>182</v>
       </c>
@@ -8917,7 +8938,7 @@
         <v>307697.18539163301</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
         <v>186</v>
       </c>
@@ -9012,7 +9033,7 @@
         <v>-605882.56941905105</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
         <v>190</v>
       </c>
@@ -9107,7 +9128,7 @@
         <v>-495967.65388783498</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
         <v>194</v>
       </c>
@@ -9202,7 +9223,7 @@
         <v>-539582.46726794203</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
         <v>200</v>
       </c>
@@ -9297,7 +9318,7 @@
         <v>-1230746.2079352699</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>204</v>
       </c>
@@ -9392,7 +9413,7 @@
         <v>400118.50166077801</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>208</v>
       </c>
@@ -9487,7 +9508,7 @@
         <v>-778499.36126290995</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
         <v>213</v>
       </c>
@@ -9582,7 +9603,7 @@
         <v>-670749.17362191598</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
         <v>218</v>
       </c>
@@ -9677,7 +9698,7 @@
         <v>117484.33535341499</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
         <v>223</v>
       </c>
@@ -9772,7 +9793,7 @@
         <v>-293464.12771677598</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
         <v>228</v>
       </c>
@@ -9867,7 +9888,7 @@
         <v>-324859.55805043399</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
         <v>233</v>
       </c>
@@ -9962,7 +9983,7 @@
         <v>-557955.86891314597</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>237</v>
       </c>
@@ -10057,7 +10078,7 @@
         <v>118904.00680124501</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
         <v>242</v>
       </c>
@@ -10152,7 +10173,7 @@
         <v>-730583.33916331304</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
         <v>247</v>
       </c>
@@ -10247,7 +10268,7 @@
         <v>-399610.78343201103</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
         <v>253</v>
       </c>
@@ -10342,7 +10363,7 @@
         <v>-471004.77694926498</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
         <v>257</v>
       </c>
@@ -10437,7 +10458,7 @@
         <v>304340.43511493102</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
         <v>260</v>
       </c>
@@ -10532,7 +10553,7 @@
         <v>-930255.40654354799</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
         <v>265</v>
       </c>
@@ -10627,7 +10648,7 @@
         <v>-444157.21427360998</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
         <v>270</v>
       </c>
@@ -10722,7 +10743,7 @@
         <v>-613355.46782811405</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
         <v>291</v>
       </c>
@@ -10823,7 +10844,7 @@
         <v>-196750.13058137</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
         <v>296</v>
       </c>
@@ -10927,7 +10948,7 @@
         <v>-748520.76591063105</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
         <v>274</v>
       </c>
@@ -11028,7 +11049,7 @@
         <v>415309.43800351198</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
         <v>281</v>
       </c>
@@ -11129,7 +11150,7 @@
         <v>480595.66509791702</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
         <v>286</v>
       </c>
@@ -11227,7 +11248,7 @@
         <v>344747.45181207301</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
         <v>301</v>
       </c>
@@ -11331,7 +11352,7 @@
         <v>463256.12167671497</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
         <v>305</v>
       </c>
@@ -11426,7 +11447,7 @@
         <v>-1262635.4183270601</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
         <v>308</v>
       </c>
@@ -11527,7 +11548,7 @@
         <v>817724.527352173</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
         <v>318</v>
       </c>
@@ -11628,7 +11649,7 @@
         <v>664174.34640780895</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
         <v>323</v>
       </c>
@@ -11729,7 +11750,7 @@
         <v>694096.87953251798</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
         <v>329</v>
       </c>
@@ -11833,7 +11854,7 @@
         <v>489316.24384795001</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
         <v>337</v>
       </c>
@@ -11937,7 +11958,7 @@
         <v>467822.17559325002</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
         <v>343</v>
       </c>
@@ -12041,7 +12062,7 @@
         <v>585569.92360688897</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
         <v>348</v>
       </c>
@@ -12145,7 +12166,7 @@
         <v>759373.17503887904</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
         <v>354</v>
       </c>
@@ -12240,7 +12261,7 @@
         <v>740287.28321332205</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
         <v>358</v>
       </c>
@@ -12335,7 +12356,7 @@
         <v>746936.49211273203</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
         <v>363</v>
       </c>
@@ -12430,7 +12451,7 @@
         <v>487619.51671457</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
         <v>367</v>
       </c>
@@ -12525,7 +12546,7 @@
         <v>583635.85127643996</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
         <v>371</v>
       </c>
@@ -12620,7 +12641,7 @@
         <v>763267.42399237503</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
         <v>386</v>
       </c>
@@ -12721,7 +12742,7 @@
         <v>739418.26488202601</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
         <v>376</v>
       </c>
@@ -12822,7 +12843,7 @@
         <v>732580.95746592898</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
         <v>382</v>
       </c>
@@ -12923,7 +12944,7 @@
         <v>820248.38406921003</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
         <v>392</v>
       </c>
@@ -13027,7 +13048,7 @@
         <v>767170.33081897604</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
         <v>398</v>
       </c>
@@ -13128,7 +13149,7 @@
         <v>1220533.29546624</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
         <v>407</v>
       </c>
@@ -13229,7 +13250,7 @@
         <v>1031554.38210208</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
         <v>414</v>
       </c>
@@ -13333,7 +13354,7 @@
         <v>808849.89977946004</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
         <v>422</v>
       </c>
@@ -13437,7 +13458,7 @@
         <v>669895.57832671201</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
         <v>427</v>
       </c>
@@ -13538,7 +13559,7 @@
         <v>1230126.4048546599</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
         <v>432</v>
       </c>
@@ -13642,7 +13663,7 @@
         <v>1278287.46153694</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>444</v>
       </c>
@@ -13740,7 +13761,7 @@
         <v>1241229.8609273101</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>450</v>
       </c>
@@ -13838,7 +13859,7 @@
         <v>936609.21582256001</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>438</v>
       </c>
@@ -13942,7 +13963,7 @@
         <v>726225.76413452905</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
         <v>461</v>
       </c>
@@ -14046,7 +14067,7 @@
         <v>1263621.0028198599</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>467</v>
       </c>
@@ -14150,7 +14171,7 @@
         <v>1042275.74376944</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
         <v>455</v>
       </c>
@@ -14251,7 +14272,7 @@
         <v>907715.48523840006</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
         <v>483</v>
       </c>
@@ -14355,7 +14376,7 @@
         <v>643994.40828936896</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
         <v>473</v>
       </c>
@@ -14456,7 +14477,7 @@
         <v>860671.81626324402</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
         <v>479</v>
       </c>
@@ -14551,7 +14572,7 @@
         <v>785629.46510451997</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
         <v>504</v>
       </c>
@@ -14655,7 +14676,7 @@
         <v>282087.35932018299</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
         <v>489</v>
       </c>
@@ -14756,7 +14777,7 @@
         <v>211983.65225900599</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
         <v>498</v>
       </c>
@@ -14860,7 +14881,7 @@
         <v>-95360.234151008495</v>
       </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
         <v>509</v>
       </c>
@@ -14955,7 +14976,7 @@
         <v>-314425.78389276197</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
         <v>513</v>
       </c>
@@ -15050,7 +15071,7 @@
         <v>45008.400596618601</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
         <v>519</v>
       </c>
@@ -15145,7 +15166,7 @@
         <v>171131.247079867</v>
       </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
         <v>523</v>
       </c>
@@ -15240,7 +15261,7 @@
         <v>-381487.79559447302</v>
       </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
         <v>527</v>
       </c>
@@ -15335,7 +15356,7 @@
         <v>-86423.985910870993</v>
       </c>
     </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
         <v>532</v>
       </c>
@@ -15430,7 +15451,7 @@
         <v>404218.16892519599</v>
       </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1" t="s">
         <v>537</v>
       </c>
@@ -15525,7 +15546,7 @@
         <v>57525.303227861397</v>
       </c>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
         <v>542</v>
       </c>
@@ -15620,7 +15641,7 @@
         <v>-356182.09145668201</v>
       </c>
     </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
         <v>547</v>
       </c>
@@ -15715,7 +15736,7 @@
         <v>-434840.92955546698</v>
       </c>
     </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
         <v>551</v>
       </c>
@@ -15810,7 +15831,7 @@
         <v>123409.229966121</v>
       </c>
     </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1" t="s">
         <v>556</v>
       </c>
@@ -15902,7 +15923,7 @@
         <v>20742.708858677099</v>
       </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1" t="s">
         <v>561</v>
       </c>
@@ -15997,7 +16018,7 @@
         <v>-310938.45683199802</v>
       </c>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1" t="s">
         <v>566</v>
       </c>
@@ -16092,7 +16113,7 @@
         <v>-439994.845335458</v>
       </c>
     </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1" t="s">
         <v>583</v>
       </c>
@@ -16193,7 +16214,7 @@
         <v>-141328.72638386299</v>
       </c>
     </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1" t="s">
         <v>575</v>
       </c>
@@ -16294,7 +16315,7 @@
         <v>-341014.35357762501</v>
       </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
         <v>570</v>
       </c>
@@ -16395,7 +16416,7 @@
         <v>30102.267323669901</v>
       </c>
     </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1" t="s">
         <v>579</v>
       </c>
@@ -16496,7 +16517,7 @@
         <v>254178.51667181501</v>
       </c>
     </row>
-    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1" t="s">
         <v>587</v>
       </c>
@@ -16600,7 +16621,7 @@
         <v>-179679.27094028</v>
       </c>
     </row>
-    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1" t="s">
         <v>592</v>
       </c>
@@ -16704,7 +16725,7 @@
         <v>375247.60853507998</v>
       </c>
     </row>
-    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1" t="s">
         <v>597</v>
       </c>
@@ -16799,7 +16820,7 @@
         <v>342555.23597454</v>
       </c>
     </row>
-    <row r="106" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1" t="s">
         <v>602</v>
       </c>
@@ -16894,7 +16915,7 @@
         <v>-21377.405480166799</v>
       </c>
     </row>
-    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1" t="s">
         <v>607</v>
       </c>
@@ -16989,7 +17010,7 @@
         <v>-188796.99880847</v>
       </c>
     </row>
-    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1" t="s">
         <v>611</v>
       </c>
@@ -17084,7 +17105,7 @@
         <v>546388.05049276596</v>
       </c>
     </row>
-    <row r="109" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1" t="s">
         <v>617</v>
       </c>
@@ -17179,7 +17200,7 @@
         <v>323074.11532936897</v>
       </c>
     </row>
-    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1" t="s">
         <v>622</v>
       </c>
@@ -17274,7 +17295,7 @@
         <v>461947.83808978199</v>
       </c>
     </row>
-    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1" t="s">
         <v>627</v>
       </c>
@@ -17369,7 +17390,7 @@
         <v>-187707.36161158999</v>
       </c>
     </row>
-    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1" t="s">
         <v>632</v>
       </c>
@@ -17464,7 +17485,7 @@
         <v>558858.90652431198</v>
       </c>
     </row>
-    <row r="113" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="1" t="s">
         <v>636</v>
       </c>
@@ -17559,7 +17580,7 @@
         <v>188760.27843670701</v>
       </c>
     </row>
-    <row r="114" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="1" t="s">
         <v>641</v>
       </c>
@@ -17654,7 +17675,7 @@
         <v>426349.60888539703</v>
       </c>
     </row>
-    <row r="115" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1" t="s">
         <v>646</v>
       </c>
@@ -17749,7 +17770,7 @@
         <v>-14436.2078329203</v>
       </c>
     </row>
-    <row r="116" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="1" t="s">
         <v>651</v>
       </c>
@@ -17844,7 +17865,7 @@
         <v>381111.62723765802</v>
       </c>
     </row>
-    <row r="117" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="1" t="s">
         <v>656</v>
       </c>
@@ -17945,7 +17966,7 @@
         <v>236879.945495908</v>
       </c>
     </row>
-    <row r="118" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1" t="s">
         <v>661</v>
       </c>
@@ -18049,7 +18070,7 @@
         <v>-323770.10159881797</v>
       </c>
     </row>
-    <row r="119" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1" t="s">
         <v>666</v>
       </c>
@@ -18150,7 +18171,7 @@
         <v>-70804.457810676598</v>
       </c>
     </row>
-    <row r="120" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1" t="s">
         <v>747</v>
       </c>
@@ -18254,7 +18275,7 @@
         <v>127756.420851702</v>
       </c>
     </row>
-    <row r="121" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1" t="s">
         <v>672</v>
       </c>
@@ -18349,7 +18370,7 @@
         <v>340821.820000473</v>
       </c>
     </row>
-    <row r="122" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1" t="s">
         <v>676</v>
       </c>
@@ -18444,7 +18465,7 @@
         <v>-112432.70028849501</v>
       </c>
     </row>
-    <row r="123" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1" t="s">
         <v>681</v>
       </c>
@@ -18539,7 +18560,7 @@
         <v>472351.11213468999</v>
       </c>
     </row>
-    <row r="124" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1" t="s">
         <v>685</v>
       </c>
@@ -18634,7 +18655,7 @@
         <v>77886.818232318299</v>
       </c>
     </row>
-    <row r="125" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="1" t="s">
         <v>690</v>
       </c>
@@ -18729,7 +18750,7 @@
         <v>40367.044923624002</v>
       </c>
     </row>
-    <row r="126" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1" t="s">
         <v>696</v>
       </c>
@@ -18824,7 +18845,7 @@
         <v>-194617.72983615901</v>
       </c>
     </row>
-    <row r="127" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1" t="s">
         <v>701</v>
       </c>
@@ -18919,7 +18940,7 @@
         <v>342275.42172751803</v>
       </c>
     </row>
-    <row r="128" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="1" t="s">
         <v>705</v>
       </c>
@@ -19014,7 +19035,7 @@
         <v>107259.04132115901</v>
       </c>
     </row>
-    <row r="129" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="1" t="s">
         <v>710</v>
       </c>
@@ -19109,7 +19130,7 @@
         <v>75397.001961251706</v>
       </c>
     </row>
-    <row r="130" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1" t="s">
         <v>715</v>
       </c>
@@ -19204,7 +19225,7 @@
         <v>-195201.59542340599</v>
       </c>
     </row>
-    <row r="131" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="1" t="s">
         <v>720</v>
       </c>
@@ -19299,7 +19320,7 @@
         <v>345147.01818214997</v>
       </c>
     </row>
-    <row r="132" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="1" t="s">
         <v>724</v>
       </c>
@@ -19394,7 +19415,7 @@
         <v>321017.59485479997</v>
       </c>
     </row>
-    <row r="133" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="1" t="s">
         <v>729</v>
       </c>
@@ -19489,7 +19510,7 @@
         <v>-341935.191698457</v>
       </c>
     </row>
-    <row r="134" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="1" t="s">
         <v>733</v>
       </c>
@@ -19584,7 +19605,7 @@
         <v>-166666.52764987599</v>
       </c>
     </row>
-    <row r="135" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="1" t="s">
         <v>738</v>
       </c>
@@ -19679,7 +19700,7 @@
         <v>113392.01015029001</v>
       </c>
     </row>
-    <row r="136" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="1" t="s">
         <v>742</v>
       </c>
@@ -19774,7 +19795,7 @@
         <v>242516.78754439499</v>
       </c>
     </row>
-    <row r="137" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="1" t="s">
         <v>753</v>
       </c>
@@ -19875,7 +19896,7 @@
         <v>-86244.400039150001</v>
       </c>
     </row>
-    <row r="138" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="1" t="s">
         <v>763</v>
       </c>
@@ -19979,7 +20000,7 @@
         <v>255372.55012319901</v>
       </c>
     </row>
-    <row r="139" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="1" t="s">
         <v>759</v>
       </c>
@@ -20083,7 +20104,7 @@
         <v>-114669.10818899301</v>
       </c>
     </row>
-    <row r="140" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1" t="s">
         <v>767</v>
       </c>
@@ -20178,7 +20199,7 @@
         <v>319184.68035712099</v>
       </c>
     </row>
-    <row r="141" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="1" t="s">
         <v>772</v>
       </c>
@@ -20273,7 +20294,7 @@
         <v>425571.365957623</v>
       </c>
     </row>
-    <row r="142" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1" t="s">
         <v>776</v>
       </c>
@@ -20368,7 +20389,7 @@
         <v>596157.14114178403</v>
       </c>
     </row>
-    <row r="143" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1" t="s">
         <v>780</v>
       </c>
@@ -20463,7 +20484,7 @@
         <v>370474.86058034899</v>
       </c>
     </row>
-    <row r="144" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1" t="s">
         <v>785</v>
       </c>
@@ -20558,7 +20579,7 @@
         <v>99672.145607464001</v>
       </c>
     </row>
-    <row r="145" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1" t="s">
         <v>790</v>
       </c>
@@ -20653,7 +20674,7 @@
         <v>68835.273305449606</v>
       </c>
     </row>
-    <row r="146" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1" t="s">
         <v>793</v>
       </c>
@@ -20748,7 +20769,7 @@
         <v>-227795.796155477</v>
       </c>
     </row>
-    <row r="147" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="1" t="s">
         <v>809</v>
       </c>
@@ -20852,7 +20873,7 @@
         <v>-152038.43809454201</v>
       </c>
     </row>
-    <row r="148" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="1" t="s">
         <v>797</v>
       </c>
@@ -20956,7 +20977,7 @@
         <v>-358901.15327821701</v>
       </c>
     </row>
-    <row r="149" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="1" t="s">
         <v>805</v>
       </c>
@@ -21060,7 +21081,7 @@
         <v>-149914.629623449</v>
       </c>
     </row>
-    <row r="150" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="1" t="s">
         <v>814</v>
       </c>
@@ -21161,7 +21182,7 @@
         <v>431930.984615736</v>
       </c>
     </row>
-    <row r="151" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="1" t="s">
         <v>820</v>
       </c>
@@ -21256,7 +21277,7 @@
         <v>340746.25331603701</v>
       </c>
     </row>
-    <row r="152" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1" t="s">
         <v>826</v>
       </c>
@@ -21351,7 +21372,7 @@
         <v>292083.35437681602</v>
       </c>
     </row>
-    <row r="153" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1" t="s">
         <v>831</v>
       </c>
@@ -21446,7 +21467,7 @@
         <v>-421008.79077386501</v>
       </c>
     </row>
-    <row r="154" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1" t="s">
         <v>836</v>
       </c>
@@ -21541,7 +21562,7 @@
         <v>-283718.74822197697</v>
       </c>
     </row>
-    <row r="155" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1" t="s">
         <v>840</v>
       </c>
@@ -21636,7 +21657,7 @@
         <v>-76603.9558039689</v>
       </c>
     </row>
-    <row r="156" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1" t="s">
         <v>845</v>
       </c>
@@ -21740,7 +21761,7 @@
         <v>521012.07005625003</v>
       </c>
     </row>
-    <row r="157" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1" t="s">
         <v>856</v>
       </c>
@@ -21838,7 +21859,7 @@
         <v>354840.03340685001</v>
       </c>
     </row>
-    <row r="158" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1" t="s">
         <v>851</v>
       </c>
@@ -21939,7 +21960,7 @@
         <v>-165030.72959307401</v>
       </c>
     </row>
-    <row r="159" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1" t="s">
         <v>862</v>
       </c>
@@ -22040,7 +22061,7 @@
         <v>-546269.39225531602</v>
       </c>
     </row>
-    <row r="160" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1" t="s">
         <v>889</v>
       </c>
@@ -22144,7 +22165,7 @@
         <v>269281.55183586403</v>
       </c>
     </row>
-    <row r="161" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="1" t="s">
         <v>868</v>
       </c>
@@ -22239,7 +22260,7 @@
         <v>-537037.05716567498</v>
       </c>
     </row>
-    <row r="162" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="1" t="s">
         <v>873</v>
       </c>
@@ -22334,7 +22355,7 @@
         <v>490011.55226499401</v>
       </c>
     </row>
-    <row r="163" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="1" t="s">
         <v>877</v>
       </c>
@@ -22429,7 +22450,7 @@
         <v>-193364.91100805701</v>
       </c>
     </row>
-    <row r="164" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1" t="s">
         <v>881</v>
       </c>
@@ -22524,7 +22545,7 @@
         <v>-270238.67560728901</v>
       </c>
     </row>
-    <row r="165" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="1" t="s">
         <v>885</v>
       </c>
@@ -22619,7 +22640,7 @@
         <v>-853040.56573804095</v>
       </c>
     </row>
-    <row r="166" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="1" t="s">
         <v>905</v>
       </c>
@@ -22720,7 +22741,7 @@
         <v>374992.95853439003</v>
       </c>
     </row>
-    <row r="167" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1" t="s">
         <v>900</v>
       </c>
@@ -22821,7 +22842,7 @@
         <v>206194.59189758901</v>
       </c>
     </row>
-    <row r="168" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1" t="s">
         <v>894</v>
       </c>
@@ -22925,7 +22946,7 @@
         <v>-222765.248903206</v>
       </c>
     </row>
-    <row r="169" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1" t="s">
         <v>908</v>
       </c>
@@ -23020,7 +23041,7 @@
         <v>-196571.08926356299</v>
       </c>
     </row>
-    <row r="170" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1" t="s">
         <v>913</v>
       </c>
@@ -23115,7 +23136,7 @@
         <v>385667.69392417802</v>
       </c>
     </row>
-    <row r="171" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1" t="s">
         <v>917</v>
       </c>
@@ -23210,7 +23231,7 @@
         <v>-657657.36204489402</v>
       </c>
     </row>
-    <row r="172" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="1" t="s">
         <v>922</v>
       </c>
@@ -23305,7 +23326,7 @@
         <v>-218866.120797821</v>
       </c>
     </row>
-    <row r="173" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="1" t="s">
         <v>926</v>
       </c>
@@ -23400,7 +23421,7 @@
         <v>-248120.59791966199</v>
       </c>
     </row>
-    <row r="174" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="1" t="s">
         <v>930</v>
       </c>
@@ -23495,7 +23516,7 @@
         <v>480830.98521926702</v>
       </c>
     </row>
-    <row r="175" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="1" t="s">
         <v>935</v>
       </c>
@@ -23590,7 +23611,7 @@
         <v>-436027.93200252199</v>
       </c>
     </row>
-    <row r="176" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="1" t="s">
         <v>940</v>
       </c>
@@ -23685,7 +23706,7 @@
         <v>-168481.59781990401</v>
       </c>
     </row>
-    <row r="177" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1" t="s">
         <v>945</v>
       </c>
@@ -23780,7 +23801,7 @@
         <v>-609526.02720464102</v>
       </c>
     </row>
-    <row r="178" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1" t="s">
         <v>950</v>
       </c>
@@ -23875,7 +23896,7 @@
         <v>19784.2791101355</v>
       </c>
     </row>
-    <row r="179" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1" t="s">
         <v>955</v>
       </c>
@@ -23970,7 +23991,7 @@
         <v>-255491.14307765701</v>
       </c>
     </row>
-    <row r="180" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1" t="s">
         <v>959</v>
       </c>
@@ -24065,7 +24086,7 @@
         <v>-34460.805079985403</v>
       </c>
     </row>
-    <row r="181" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="1" t="s">
         <v>964</v>
       </c>
@@ -24160,7 +24181,7 @@
         <v>-509593.068635837</v>
       </c>
     </row>
-    <row r="182" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1" t="s">
         <v>969</v>
       </c>
@@ -24255,7 +24276,7 @@
         <v>-225015.008700487</v>
       </c>
     </row>
-    <row r="183" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1" t="s">
         <v>972</v>
       </c>
@@ -24350,7 +24371,7 @@
         <v>-521457.73443066701</v>
       </c>
     </row>
-    <row r="184" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1" t="s">
         <v>981</v>
       </c>
@@ -24451,7 +24472,7 @@
         <v>-373050.49283215799</v>
       </c>
     </row>
-    <row r="185" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1" t="s">
         <v>977</v>
       </c>
@@ -24552,7 +24573,7 @@
         <v>-308795.39965818898</v>
       </c>
     </row>
-    <row r="186" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1" t="s">
         <v>986</v>
       </c>
@@ -24650,7 +24671,7 @@
         <v>-133921.54810268001</v>
       </c>
     </row>
-    <row r="187" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1" t="s">
         <v>991</v>
       </c>
@@ -24754,7 +24775,7 @@
         <v>326769.80347670399</v>
       </c>
     </row>
-    <row r="188" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1" t="s">
         <v>996</v>
       </c>
@@ -24855,7 +24876,7 @@
         <v>-155644.912342884</v>
       </c>
     </row>
-    <row r="189" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1" t="s">
         <v>1005</v>
       </c>
@@ -24959,7 +24980,7 @@
         <v>-68091.835581703999</v>
       </c>
     </row>
-    <row r="190" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1" t="s">
         <v>1001</v>
       </c>
@@ -25054,7 +25075,7 @@
         <v>316569.01359511999</v>
       </c>
     </row>
-    <row r="191" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1" t="s">
         <v>1011</v>
       </c>
@@ -25158,7 +25179,7 @@
         <v>-88951.145354809894</v>
       </c>
     </row>
-    <row r="192" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="1" t="s">
         <v>1018</v>
       </c>
@@ -25259,7 +25280,7 @@
         <v>370282.52070736</v>
       </c>
     </row>
-    <row r="193" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="1" t="s">
         <v>1024</v>
       </c>
@@ -25357,7 +25378,7 @@
         <v>402610.972602978</v>
       </c>
     </row>
-    <row r="194" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="1" t="s">
         <v>1075</v>
       </c>
@@ -25455,7 +25476,7 @@
         <v>42965.671097610102</v>
       </c>
     </row>
-    <row r="195" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="1" t="s">
         <v>1069</v>
       </c>
@@ -25553,7 +25574,7 @@
         <v>166954.17369700299</v>
       </c>
     </row>
-    <row r="196" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="1" t="s">
         <v>1063</v>
       </c>
@@ -25657,7 +25678,7 @@
         <v>465804.83905814099</v>
       </c>
     </row>
-    <row r="197" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="1" t="s">
         <v>1029</v>
       </c>
@@ -25752,7 +25773,7 @@
         <v>404566.60879252298</v>
       </c>
     </row>
-    <row r="198" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="1" t="s">
         <v>1033</v>
       </c>
@@ -25847,7 +25868,7 @@
         <v>168597.78356868701</v>
       </c>
     </row>
-    <row r="199" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="1" t="s">
         <v>1037</v>
       </c>
@@ -25942,7 +25963,7 @@
         <v>405749.81587815098</v>
       </c>
     </row>
-    <row r="200" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="1" t="s">
         <v>1040</v>
       </c>
@@ -26037,7 +26058,7 @@
         <v>303992.99579951202</v>
       </c>
     </row>
-    <row r="201" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="1" t="s">
         <v>1044</v>
       </c>
@@ -26132,7 +26153,7 @@
         <v>451093.92103917</v>
       </c>
     </row>
-    <row r="202" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="1" t="s">
         <v>1049</v>
       </c>
@@ -26227,7 +26248,7 @@
         <v>157968.36181606699</v>
       </c>
     </row>
-    <row r="203" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="1" t="s">
         <v>1054</v>
       </c>
@@ -26322,7 +26343,7 @@
         <v>514980.39186726301</v>
       </c>
     </row>
-    <row r="204" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="1" t="s">
         <v>1058</v>
       </c>
@@ -26417,7 +26438,7 @@
         <v>291113.30045480002</v>
       </c>
     </row>
-    <row r="205" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="1" t="s">
         <v>1086</v>
       </c>
@@ -26521,7 +26542,7 @@
         <v>492476.92035953997</v>
       </c>
     </row>
-    <row r="206" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="1" t="s">
         <v>1091</v>
       </c>
@@ -26625,7 +26646,7 @@
         <v>487973.03618982801</v>
       </c>
     </row>
-    <row r="207" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="1" t="s">
         <v>1080</v>
       </c>
@@ -26729,7 +26750,7 @@
         <v>187457.910664939</v>
       </c>
     </row>
-    <row r="208" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="1" t="s">
         <v>1096</v>
       </c>
@@ -26833,7 +26854,7 @@
         <v>352690.58614449803</v>
       </c>
     </row>
-    <row r="209" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="1" t="s">
         <v>1101</v>
       </c>
@@ -26937,7 +26958,7 @@
         <v>368154.88059001003</v>
       </c>
     </row>
-    <row r="210" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="1" t="s">
         <v>1107</v>
       </c>
@@ -27041,7 +27062,7 @@
         <v>22455.230780900001</v>
       </c>
     </row>
-    <row r="211" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="1" t="s">
         <v>1111</v>
       </c>
@@ -27142,7 +27163,7 @@
         <v>463023.04977379797</v>
       </c>
     </row>
-    <row r="212" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="1" t="s">
         <v>1115</v>
       </c>
@@ -27246,7 +27267,7 @@
         <v>336998.95526081201</v>
       </c>
     </row>
-    <row r="213" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="1" t="s">
         <v>1119</v>
       </c>
@@ -27344,7 +27365,7 @@
         <v>35990.000437881703</v>
       </c>
     </row>
-    <row r="214" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="1" t="s">
         <v>1195</v>
       </c>
@@ -27442,7 +27463,7 @@
         <v>336364.91468164901</v>
       </c>
     </row>
-    <row r="215" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="1" t="s">
         <v>1189</v>
       </c>
@@ -27546,7 +27567,7 @@
         <v>328387.82288657298</v>
       </c>
     </row>
-    <row r="216" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="1" t="s">
         <v>1124</v>
       </c>
@@ -27641,7 +27662,7 @@
         <v>395385.26082271599</v>
       </c>
     </row>
-    <row r="217" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="1" t="s">
         <v>1129</v>
       </c>
@@ -27736,7 +27757,7 @@
         <v>70200.329942488097</v>
       </c>
     </row>
-    <row r="218" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="1" t="s">
         <v>1133</v>
       </c>
@@ -27831,7 +27852,7 @@
         <v>291954.81959152798</v>
       </c>
     </row>
-    <row r="219" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="1" t="s">
         <v>1138</v>
       </c>
@@ -27926,7 +27947,7 @@
         <v>251746.317477192</v>
       </c>
     </row>
-    <row r="220" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="1" t="s">
         <v>1142</v>
       </c>
@@ -28021,7 +28042,7 @@
         <v>479208.17282562598</v>
       </c>
     </row>
-    <row r="221" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="1" t="s">
         <v>1147</v>
       </c>
@@ -28116,7 +28137,7 @@
         <v>108261.53799623701</v>
       </c>
     </row>
-    <row r="222" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="1" t="s">
         <v>1150</v>
       </c>
@@ -28211,7 +28232,7 @@
         <v>400487.55141714402</v>
       </c>
     </row>
-    <row r="223" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="1" t="s">
         <v>1154</v>
       </c>
@@ -28306,7 +28327,7 @@
         <v>175575.05791926401</v>
       </c>
     </row>
-    <row r="224" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="1" t="s">
         <v>1158</v>
       </c>
@@ -28401,7 +28422,7 @@
         <v>361063.74818921502</v>
       </c>
     </row>
-    <row r="225" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="1" t="s">
         <v>1163</v>
       </c>
@@ -28496,7 +28517,7 @@
         <v>215571.61772622401</v>
       </c>
     </row>
-    <row r="226" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="1" t="s">
         <v>1167</v>
       </c>
@@ -28591,7 +28612,7 @@
         <v>435542.812967612</v>
       </c>
     </row>
-    <row r="227" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="1" t="s">
         <v>1170</v>
       </c>
@@ -28686,7 +28707,7 @@
         <v>177563.48811663999</v>
       </c>
     </row>
-    <row r="228" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="1" t="s">
         <v>1175</v>
       </c>
@@ -28781,7 +28802,7 @@
         <v>372430.41975373798</v>
       </c>
     </row>
-    <row r="229" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="1" t="s">
         <v>1180</v>
       </c>
@@ -28876,7 +28897,7 @@
         <v>405029.73521196702</v>
       </c>
     </row>
-    <row r="230" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="1" t="s">
         <v>1184</v>
       </c>
@@ -28971,7 +28992,7 @@
         <v>362136.86742162198</v>
       </c>
     </row>
-    <row r="231" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="1" t="s">
         <v>1209</v>
       </c>
@@ -29075,7 +29096,7 @@
         <v>115899.452144499</v>
       </c>
     </row>
-    <row r="232" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="1" t="s">
         <v>1200</v>
       </c>
@@ -29176,7 +29197,7 @@
         <v>893641.02619626501</v>
       </c>
     </row>
-    <row r="233" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="1" t="s">
         <v>1205</v>
       </c>
@@ -29277,7 +29298,7 @@
         <v>1150985.9530076301</v>
       </c>
     </row>
-    <row r="234" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="1" t="s">
         <v>1227</v>
       </c>
@@ -29378,7 +29399,7 @@
         <v>698379.77909993695</v>
       </c>
     </row>
-    <row r="235" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="1" t="s">
         <v>1214</v>
       </c>
@@ -29479,7 +29500,7 @@
         <v>547139.06522827002</v>
       </c>
     </row>
-    <row r="236" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="1" t="s">
         <v>1222</v>
       </c>
@@ -29580,7 +29601,7 @@
         <v>496298.42609967</v>
       </c>
     </row>
-    <row r="237" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="1" t="s">
         <v>1233</v>
       </c>
@@ -29681,7 +29702,7 @@
         <v>642523.38573941495</v>
       </c>
     </row>
-    <row r="238" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="1" t="s">
         <v>1239</v>
       </c>
@@ -29782,7 +29803,7 @@
         <v>686645.42044066999</v>
       </c>
     </row>
-    <row r="239" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="1" t="s">
         <v>1259</v>
       </c>
@@ -29886,7 +29907,7 @@
         <v>925476.26648929296</v>
       </c>
     </row>
-    <row r="240" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="1" t="s">
         <v>1252</v>
       </c>
@@ -29990,7 +30011,7 @@
         <v>1004970.98272945</v>
       </c>
     </row>
-    <row r="241" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="1" t="s">
         <v>1244</v>
       </c>
@@ -30091,7 +30112,7 @@
         <v>725507.19012757705</v>
       </c>
     </row>
-    <row r="242" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="1" t="s">
         <v>1264</v>
       </c>
@@ -30186,7 +30207,7 @@
         <v>873074.98588307004</v>
       </c>
     </row>
-    <row r="243" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="1" t="s">
         <v>1269</v>
       </c>
@@ -30281,7 +30302,7 @@
         <v>-91693.299208712706</v>
       </c>
     </row>
-    <row r="244" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="1" t="s">
         <v>1274</v>
       </c>
@@ -30376,7 +30397,7 @@
         <v>557960.74881765002</v>
       </c>
     </row>
-    <row r="245" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="1" t="s">
         <v>1285</v>
       </c>
@@ -30477,7 +30498,7 @@
         <v>381910.40398969001</v>
       </c>
     </row>
-    <row r="246" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="1" t="s">
         <v>1280</v>
       </c>
@@ -30578,7 +30599,7 @@
         <v>963965.57805772906</v>
       </c>
     </row>
-    <row r="247" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="1" t="s">
         <v>1293</v>
       </c>
@@ -30676,7 +30697,7 @@
         <v>1196331.7397851499</v>
       </c>
     </row>
-    <row r="248" spans="1:35" ht="29.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:35" ht="29.85" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="1" t="s">
         <v>1356</v>
       </c>
@@ -30780,7 +30801,7 @@
         <v>-37329.3055729353</v>
       </c>
     </row>
-    <row r="249" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="1" t="s">
         <v>1299</v>
       </c>
@@ -30881,7 +30902,7 @@
         <v>468823.13934554998</v>
       </c>
     </row>
-    <row r="250" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="1" t="s">
         <v>1373</v>
       </c>
@@ -30985,7 +31006,7 @@
         <v>824871.87805665005</v>
       </c>
     </row>
-    <row r="251" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="1" t="s">
         <v>1362</v>
       </c>
@@ -31089,7 +31110,7 @@
         <v>1085839.94245835</v>
       </c>
     </row>
-    <row r="252" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="1" t="s">
         <v>1305</v>
       </c>
@@ -31184,7 +31205,7 @@
         <v>650009.061604394</v>
       </c>
     </row>
-    <row r="253" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="1" t="s">
         <v>1310</v>
       </c>
@@ -31279,7 +31300,7 @@
         <v>448539.75168605801</v>
       </c>
     </row>
-    <row r="254" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="1" t="s">
         <v>1368</v>
       </c>
@@ -31383,7 +31404,7 @@
         <v>1007843.29880446</v>
       </c>
     </row>
-    <row r="255" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="1" t="s">
         <v>1314</v>
       </c>
@@ -31475,7 +31496,7 @@
         <v>1127854.3412725099</v>
       </c>
     </row>
-    <row r="256" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="1" t="s">
         <v>1317</v>
       </c>
@@ -31570,7 +31591,7 @@
         <v>-205502.237967669</v>
       </c>
     </row>
-    <row r="257" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="1" t="s">
         <v>1323</v>
       </c>
@@ -31665,7 +31686,7 @@
         <v>171797.05432159899</v>
       </c>
     </row>
-    <row r="258" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="1" t="s">
         <v>1328</v>
       </c>
@@ -31760,7 +31781,7 @@
         <v>488312.64038407098</v>
       </c>
     </row>
-    <row r="259" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="1" t="s">
         <v>1333</v>
       </c>
@@ -31855,7 +31876,7 @@
         <v>233291.15342406699</v>
       </c>
     </row>
-    <row r="260" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="1" t="s">
         <v>1338</v>
       </c>
@@ -31950,7 +31971,7 @@
         <v>-238805.64801191</v>
       </c>
     </row>
-    <row r="261" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="1" t="s">
         <v>1343</v>
       </c>
@@ -32045,7 +32066,7 @@
         <v>934048.87102714705</v>
       </c>
     </row>
-    <row r="262" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" s="1" t="s">
         <v>1347</v>
       </c>
@@ -32140,7 +32161,7 @@
         <v>1521054.9437484799</v>
       </c>
     </row>
-    <row r="263" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="1" t="s">
         <v>1352</v>
       </c>
@@ -32235,7 +32256,7 @@
         <v>-427983.466876694</v>
       </c>
     </row>
-    <row r="264" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" s="1" t="s">
         <v>1387</v>
       </c>
@@ -32339,7 +32360,7 @@
         <v>1285915.80443856</v>
       </c>
     </row>
-    <row r="265" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" s="1" t="s">
         <v>1381</v>
       </c>
@@ -32440,7 +32461,7 @@
         <v>94154.660111314603</v>
       </c>
     </row>
-    <row r="266" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="1" t="s">
         <v>1391</v>
       </c>
@@ -32544,7 +32565,7 @@
         <v>1198985.2505878101</v>
       </c>
     </row>
-    <row r="267" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="1" t="s">
         <v>1395</v>
       </c>
@@ -32639,7 +32660,7 @@
         <v>-165062.06751099601</v>
       </c>
     </row>
-    <row r="268" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="1" t="s">
         <v>1399</v>
       </c>
@@ -32734,7 +32755,7 @@
         <v>997952.23155729705</v>
       </c>
     </row>
-    <row r="269" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="1" t="s">
         <v>1403</v>
       </c>
@@ -32829,7 +32850,7 @@
         <v>236984.95067794601</v>
       </c>
     </row>
-    <row r="270" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" s="1" t="s">
         <v>1408</v>
       </c>
@@ -32924,7 +32945,7 @@
         <v>935563.45755298401</v>
       </c>
     </row>
-    <row r="271" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="1" t="s">
         <v>1411</v>
       </c>
@@ -33016,7 +33037,7 @@
         <v>-328089.12790757598</v>
       </c>
     </row>
-    <row r="272" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" s="1" t="s">
         <v>1416</v>
       </c>
@@ -33111,7 +33132,7 @@
         <v>61419.014752710202</v>
       </c>
     </row>
-    <row r="273" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" s="1" t="s">
         <v>1421</v>
       </c>
@@ -33206,7 +33227,7 @@
         <v>131207.52796321001</v>
       </c>
     </row>
-    <row r="274" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="1" t="s">
         <v>1426</v>
       </c>
@@ -33301,7 +33322,7 @@
         <v>-108350.45835278201</v>
       </c>
     </row>
-    <row r="275" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" s="1" t="s">
         <v>1430</v>
       </c>
@@ -33396,7 +33417,7 @@
         <v>-124572.48900109901</v>
       </c>
     </row>
-    <row r="276" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" s="1" t="s">
         <v>1440</v>
       </c>
@@ -33500,7 +33521,7 @@
         <v>-195215.250386136</v>
       </c>
     </row>
-    <row r="277" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="1" t="s">
         <v>1434</v>
       </c>
@@ -33601,7 +33622,7 @@
         <v>351672.47639779799</v>
       </c>
     </row>
-    <row r="278" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="1" t="s">
         <v>1443</v>
       </c>
@@ -33699,7 +33720,7 @@
         <v>66459.077240928003</v>
       </c>
     </row>
-    <row r="279" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="1" t="s">
         <v>1477</v>
       </c>
@@ -33797,7 +33818,7 @@
         <v>724867.48494588502</v>
       </c>
     </row>
-    <row r="280" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" s="1" t="s">
         <v>1472</v>
       </c>
@@ -33895,7 +33916,7 @@
         <v>248319.26822224099</v>
       </c>
     </row>
-    <row r="281" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="1" t="s">
         <v>1449</v>
       </c>
@@ -33990,7 +34011,7 @@
         <v>1098399.30856572</v>
       </c>
     </row>
-    <row r="282" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="1" t="s">
         <v>1466</v>
       </c>
@@ -34094,7 +34115,7 @@
         <v>1106992.65421078</v>
       </c>
     </row>
-    <row r="283" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="1" t="s">
         <v>1453</v>
       </c>
@@ -34183,7 +34204,7 @@
         <v>993825.16307185299</v>
       </c>
     </row>
-    <row r="284" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="1" t="s">
         <v>1457</v>
       </c>
@@ -34278,7 +34299,7 @@
         <v>240962.44211004299</v>
       </c>
     </row>
-    <row r="285" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="1" t="s">
         <v>1462</v>
       </c>
@@ -34367,7 +34388,7 @@
         <v>1084343.5940164099</v>
       </c>
     </row>
-    <row r="286" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" s="1" t="s">
         <v>1489</v>
       </c>
@@ -34468,7 +34489,7 @@
         <v>389624.22426249803</v>
       </c>
     </row>
-    <row r="287" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="1" t="s">
         <v>1496</v>
       </c>
@@ -34569,7 +34590,7 @@
         <v>-316541.80296781298</v>
       </c>
     </row>
-    <row r="288" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="1" t="s">
         <v>1483</v>
       </c>
@@ -34673,7 +34694,7 @@
         <v>874533.0547795</v>
       </c>
     </row>
-    <row r="289" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="1" t="s">
         <v>1525</v>
       </c>
@@ -34777,7 +34798,7 @@
         <v>-323283.52678093198</v>
       </c>
     </row>
-    <row r="290" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" s="1" t="s">
         <v>1537</v>
       </c>
@@ -34875,7 +34896,7 @@
         <v>-184963.65210150799</v>
       </c>
     </row>
-    <row r="291" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="1" t="s">
         <v>1502</v>
       </c>
@@ -34976,7 +34997,7 @@
         <v>638963.61072893604</v>
       </c>
     </row>
-    <row r="292" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="1" t="s">
         <v>1531</v>
       </c>
@@ -35080,7 +35101,7 @@
         <v>342208.23570972402</v>
       </c>
     </row>
-    <row r="293" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" s="1" t="s">
         <v>1507</v>
       </c>
@@ -35175,7 +35196,7 @@
         <v>830797.96942348697</v>
       </c>
     </row>
-    <row r="294" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="1" t="s">
         <v>1512</v>
       </c>
@@ -35270,7 +35291,7 @@
         <v>-265882.80556511198</v>
       </c>
     </row>
-    <row r="295" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="1" t="s">
         <v>1516</v>
       </c>
@@ -35365,7 +35386,7 @@
         <v>709350.95875112398</v>
       </c>
     </row>
-    <row r="296" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="1" t="s">
         <v>1520</v>
       </c>
@@ -35460,7 +35481,7 @@
         <v>-589315.89379228698</v>
       </c>
     </row>
-    <row r="297" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="1" t="s">
         <v>1542</v>
       </c>
@@ -35564,7 +35585,7 @@
         <v>323951.79813845601</v>
       </c>
     </row>
-    <row r="298" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="1" t="s">
         <v>1546</v>
       </c>
@@ -35668,7 +35689,7 @@
         <v>324142.96458676597</v>
       </c>
     </row>
-    <row r="299" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="1" t="s">
         <v>1551</v>
       </c>
@@ -35769,7 +35790,7 @@
         <v>635203.29720487294</v>
       </c>
     </row>
-    <row r="300" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" s="1" t="s">
         <v>1556</v>
       </c>
@@ -35864,7 +35885,7 @@
         <v>713149.86173744395</v>
       </c>
     </row>
-    <row r="301" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" s="1" t="s">
         <v>1560</v>
       </c>
@@ -35959,7 +35980,7 @@
         <v>-27416.805160369699</v>
       </c>
     </row>
-    <row r="302" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" s="1" t="s">
         <v>1565</v>
       </c>
@@ -36054,7 +36075,7 @@
         <v>422172.10182119999</v>
       </c>
     </row>
-    <row r="303" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" s="1" t="s">
         <v>1618</v>
       </c>
@@ -36158,7 +36179,7 @@
         <v>660641.07549193001</v>
       </c>
     </row>
-    <row r="304" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" s="1" t="s">
         <v>1570</v>
       </c>
@@ -36253,7 +36274,7 @@
         <v>505348.28455864399</v>
       </c>
     </row>
-    <row r="305" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" s="1" t="s">
         <v>1575</v>
       </c>
@@ -36348,7 +36369,7 @@
         <v>1372930.1275132301</v>
       </c>
     </row>
-    <row r="306" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" s="1" t="s">
         <v>1579</v>
       </c>
@@ -36443,7 +36464,7 @@
         <v>600220.95442781504</v>
       </c>
     </row>
-    <row r="307" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" s="1" t="s">
         <v>1582</v>
       </c>
@@ -36538,7 +36559,7 @@
         <v>779532.82962748501</v>
       </c>
     </row>
-    <row r="308" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" s="1" t="s">
         <v>1586</v>
       </c>
@@ -36633,7 +36654,7 @@
         <v>-281535.253722461</v>
       </c>
     </row>
-    <row r="309" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" s="1" t="s">
         <v>1622</v>
       </c>
@@ -36737,7 +36758,7 @@
         <v>1392540.17553827</v>
       </c>
     </row>
-    <row r="310" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" s="1" t="s">
         <v>1590</v>
       </c>
@@ -36832,7 +36853,7 @@
         <v>576243.09663408704</v>
       </c>
     </row>
-    <row r="311" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" s="1" t="s">
         <v>1594</v>
       </c>
@@ -36927,7 +36948,7 @@
         <v>547250.91681603505</v>
       </c>
     </row>
-    <row r="312" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" s="1" t="s">
         <v>1599</v>
       </c>
@@ -37022,7 +37043,7 @@
         <v>-575193.11328341998</v>
       </c>
     </row>
-    <row r="313" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" s="1" t="s">
         <v>1603</v>
       </c>
@@ -37114,7 +37135,7 @@
         <v>451032.19933941402</v>
       </c>
     </row>
-    <row r="314" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" s="1" t="s">
         <v>1607</v>
       </c>
@@ -37209,7 +37230,7 @@
         <v>713172.77936673001</v>
       </c>
     </row>
-    <row r="315" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" s="1" t="s">
         <v>1610</v>
       </c>
@@ -37304,7 +37325,7 @@
         <v>632567.87179277802</v>
       </c>
     </row>
-    <row r="316" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" s="1" t="s">
         <v>1614</v>
       </c>
@@ -37399,7 +37420,7 @@
         <v>-124682.62151569199</v>
       </c>
     </row>
-    <row r="317" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" s="1" t="s">
         <v>1627</v>
       </c>
@@ -37503,7 +37524,7 @@
         <v>-357345.93663740897</v>
       </c>
     </row>
-    <row r="318" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" s="1" t="s">
         <v>1633</v>
       </c>
@@ -37607,7 +37628,7 @@
         <v>407599.34133697202</v>
       </c>
     </row>
-    <row r="319" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" s="1" t="s">
         <v>1638</v>
       </c>
@@ -37705,7 +37726,7 @@
         <v>665568.98532973405</v>
       </c>
     </row>
-    <row r="320" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" s="1" t="s">
         <v>1643</v>
       </c>
@@ -37800,7 +37821,7 @@
         <v>1291773.8336334201</v>
       </c>
     </row>
-    <row r="321" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" s="1" t="s">
         <v>1648</v>
       </c>
@@ -37895,7 +37916,7 @@
         <v>629571.77291901805</v>
       </c>
     </row>
-    <row r="322" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" s="1" t="s">
         <v>1653</v>
       </c>
@@ -37990,7 +38011,7 @@
         <v>1287345.0869581599</v>
       </c>
     </row>
-    <row r="323" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" s="1" t="s">
         <v>1656</v>
       </c>
@@ -38082,7 +38103,7 @@
         <v>276298.73528388399</v>
       </c>
     </row>
-    <row r="324" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="1" t="s">
         <v>1669</v>
       </c>
@@ -38186,7 +38207,7 @@
         <v>793971.23601419805</v>
       </c>
     </row>
-    <row r="325" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="1" t="s">
         <v>1661</v>
       </c>
@@ -38281,7 +38302,7 @@
         <v>384747.32127326902</v>
       </c>
     </row>
-    <row r="326" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" s="1" t="s">
         <v>1664</v>
       </c>
@@ -38376,7 +38397,7 @@
         <v>437867.96990440402</v>
       </c>
     </row>
-    <row r="327" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" s="1" t="s">
         <v>1679</v>
       </c>
@@ -38480,7 +38501,7 @@
         <v>345373.564749729</v>
       </c>
     </row>
-    <row r="328" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" s="1" t="s">
         <v>1683</v>
       </c>
@@ -38584,7 +38605,7 @@
         <v>266452.56175278203</v>
       </c>
     </row>
-    <row r="329" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" s="1" t="s">
         <v>1674</v>
       </c>
@@ -38685,7 +38706,7 @@
         <v>590839.19161300303</v>
       </c>
     </row>
-    <row r="330" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" s="1" t="s">
         <v>1688</v>
       </c>
@@ -38780,7 +38801,7 @@
         <v>612172.87845144898</v>
       </c>
     </row>
-    <row r="331" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" s="1" t="s">
         <v>1693</v>
       </c>
@@ -38875,7 +38896,7 @@
         <v>198151.389220707</v>
       </c>
     </row>
-    <row r="332" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" s="1" t="s">
         <v>1718</v>
       </c>
@@ -38979,7 +39000,7 @@
         <v>743129.40021104505</v>
       </c>
     </row>
-    <row r="333" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="1" t="s">
         <v>1697</v>
       </c>
@@ -39074,7 +39095,7 @@
         <v>732017.67710272095</v>
       </c>
     </row>
-    <row r="334" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" s="1" t="s">
         <v>1701</v>
       </c>
@@ -39169,7 +39190,7 @@
         <v>46254.529440539802</v>
       </c>
     </row>
-    <row r="335" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" s="1" t="s">
         <v>1705</v>
       </c>
@@ -39264,7 +39285,7 @@
         <v>888257.74773520895</v>
       </c>
     </row>
-    <row r="336" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" s="1" t="s">
         <v>1709</v>
       </c>
@@ -39359,7 +39380,7 @@
         <v>453884.73195741</v>
       </c>
     </row>
-    <row r="337" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" s="1" t="s">
         <v>1713</v>
       </c>
@@ -39454,7 +39475,7 @@
         <v>461375.85186104599</v>
       </c>
     </row>
-    <row r="338" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" s="5" t="s">
         <v>1376</v>
       </c>
@@ -39552,7 +39573,7 @@
         <v>-372481.46087195602</v>
       </c>
     </row>
-    <row r="339" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" s="1" t="s">
         <v>1739</v>
       </c>
@@ -39593,7 +39614,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="340" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" s="1" t="s">
         <v>1773</v>
       </c>
@@ -39629,7 +39650,7 @@
         <v>-84.747316934702894</v>
       </c>
     </row>
-    <row r="341" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" s="1" t="s">
         <v>1774</v>
       </c>
@@ -39665,7 +39686,7 @@
         <v>-82.971341215743095</v>
       </c>
     </row>
-    <row r="342" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" s="1" t="s">
         <v>1775</v>
       </c>
@@ -39701,7 +39722,7 @@
         <v>-82.345119494735499</v>
       </c>
     </row>
-    <row r="343" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" s="1" t="s">
         <v>1776</v>
       </c>
@@ -39722,6 +39743,9 @@
       </c>
       <c r="K343" s="1" t="s">
         <v>136</v>
+      </c>
+      <c r="M343" s="1" t="s">
+        <v>1816</v>
       </c>
       <c r="Q343">
         <v>19387454</v>
@@ -39737,7 +39761,7 @@
         <v>-81.2520544939199</v>
       </c>
     </row>
-    <row r="344" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" s="1" t="s">
         <v>1777</v>
       </c>
@@ -39773,7 +39797,7 @@
         <v>-85.000910028763499</v>
       </c>
     </row>
-    <row r="345" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" s="1" t="s">
         <v>1778</v>
       </c>
@@ -39809,7 +39833,7 @@
         <v>-83.448027980945994</v>
       </c>
     </row>
-    <row r="346" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" s="1" t="s">
         <v>1779</v>
       </c>
@@ -39845,7 +39869,7 @@
         <v>-82.034038129835594</v>
       </c>
     </row>
-    <row r="347" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A347" s="1" t="s">
         <v>1780</v>
       </c>
@@ -39881,7 +39905,7 @@
         <v>-84.000369126963193</v>
       </c>
     </row>
-    <row r="348" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A348" s="1" t="s">
         <v>1781</v>
       </c>
@@ -39919,7 +39943,7 @@
         <v>-82.987843018393406</v>
       </c>
     </row>
-    <row r="349" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A349" s="1" t="s">
         <v>1782</v>
       </c>
@@ -39955,7 +39979,7 @@
         <v>-83.454889952360006</v>
       </c>
     </row>
-    <row r="350" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A350" s="1" t="s">
         <v>1783</v>
       </c>
@@ -39991,7 +40015,7 @@
         <v>-82.377163119041896</v>
       </c>
     </row>
-    <row r="351" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A351" s="1" t="s">
         <v>1784</v>
       </c>
@@ -40027,7 +40051,7 @@
         <v>-83.900082955875803</v>
       </c>
     </row>
-    <row r="352" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A352" s="1" t="s">
         <v>1785</v>
       </c>
@@ -40048,6 +40072,12 @@
       </c>
       <c r="K352" s="1" t="s">
         <v>136</v>
+      </c>
+      <c r="L352" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="M352" s="1" t="s">
+        <v>1126</v>
       </c>
       <c r="Q352">
         <v>5213645</v>
@@ -40063,7 +40093,7 @@
         <v>-83.048366463009998</v>
       </c>
     </row>
-    <row r="353" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" s="1" t="s">
         <v>1786</v>
       </c>
@@ -40099,7 +40129,7 @@
         <v>-82.120590150109606</v>
       </c>
     </row>
-    <row r="354" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" s="1" t="s">
         <v>1787</v>
       </c>
@@ -40135,7 +40165,7 @@
         <v>-82.473347387627499</v>
       </c>
     </row>
-    <row r="355" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" s="1" t="s">
         <v>1788</v>
       </c>
@@ -40156,6 +40186,9 @@
       </c>
       <c r="K355" s="1" t="s">
         <v>136</v>
+      </c>
+      <c r="M355" s="1" t="s">
+        <v>1815</v>
       </c>
       <c r="Q355">
         <v>3980812</v>
@@ -40171,7 +40204,7 @@
         <v>-83.966111834383796</v>
       </c>
     </row>
-    <row r="356" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" s="1" t="s">
         <v>1789</v>
       </c>
@@ -40207,7 +40240,7 @@
         <v>-82.503754203997801</v>
       </c>
     </row>
-    <row r="357" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" s="1" t="s">
         <v>1790</v>
       </c>
@@ -40228,6 +40261,9 @@
       </c>
       <c r="K357" s="1" t="s">
         <v>136</v>
+      </c>
+      <c r="M357" s="1" t="s">
+        <v>1814</v>
       </c>
       <c r="Q357">
         <v>15585938</v>
@@ -40243,7 +40279,7 @@
         <v>-81.200751030168703</v>
       </c>
     </row>
-    <row r="358" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" s="1" t="s">
         <v>1791</v>
       </c>
@@ -40264,6 +40300,9 @@
       </c>
       <c r="K358" s="1" t="s">
         <v>136</v>
+      </c>
+      <c r="M358" s="1" t="s">
+        <v>1813</v>
       </c>
       <c r="Q358">
         <v>3982320</v>
@@ -40279,7 +40318,7 @@
         <v>-84.334979346507694</v>
       </c>
     </row>
-    <row r="359" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" s="1" t="s">
         <v>1792</v>
       </c>
@@ -40315,7 +40354,7 @@
         <v>-80.9817571525235</v>
       </c>
     </row>
-    <row r="360" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A360" s="1" t="s">
         <v>1793</v>
       </c>
@@ -40351,7 +40390,7 @@
         <v>-81.187225578043694</v>
       </c>
     </row>
-    <row r="361" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A361" s="1" t="s">
         <v>1794</v>
       </c>
@@ -40387,7 +40426,7 @@
         <v>-80.823521445265598</v>
       </c>
     </row>
-    <row r="362" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A362" s="1" t="s">
         <v>1795</v>
       </c>
@@ -40408,6 +40447,9 @@
       </c>
       <c r="K362" s="1" t="s">
         <v>136</v>
+      </c>
+      <c r="M362" t="s">
+        <v>1812</v>
       </c>
       <c r="Q362">
         <v>1918274</v>
@@ -40423,7 +40465,7 @@
         <v>-83.781203046291594</v>
       </c>
     </row>
-    <row r="363" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A363" s="1" t="s">
         <v>1796</v>
       </c>
@@ -40444,6 +40486,9 @@
       </c>
       <c r="K363" s="1" t="s">
         <v>136</v>
+      </c>
+      <c r="M363" t="s">
+        <v>1811</v>
       </c>
       <c r="Q363">
         <v>13155459</v>
@@ -40459,7 +40504,7 @@
         <v>-81.169993668031907</v>
       </c>
     </row>
-    <row r="364" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A364" s="1" t="s">
         <v>1797</v>
       </c>
@@ -40495,7 +40540,7 @@
         <v>-83.386268048007196</v>
       </c>
     </row>
-    <row r="365" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A365" s="1" t="s">
         <v>1798</v>
       </c>
@@ -40531,7 +40576,7 @@
         <v>-81.186593413475407</v>
       </c>
     </row>
-    <row r="366" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A366" s="1" t="s">
         <v>1799</v>
       </c>
@@ -40567,7 +40612,7 @@
         <v>-82.326759254122095</v>
       </c>
     </row>
-    <row r="367" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A367" s="1" t="s">
         <v>1800</v>
       </c>
@@ -40603,7 +40648,7 @@
         <v>-83.478393130109495</v>
       </c>
     </row>
-    <row r="368" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A368" s="1" t="s">
         <v>1801</v>
       </c>
@@ -40639,7 +40684,7 @@
         <v>-81.370740867640194</v>
       </c>
     </row>
-    <row r="369" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A369" s="1" t="s">
         <v>1802</v>
       </c>
@@ -40675,7 +40720,7 @@
         <v>-81.196563091245594</v>
       </c>
     </row>
-    <row r="370" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A370" s="1" t="s">
         <v>1803</v>
       </c>
@@ -40711,7 +40756,7 @@
         <v>-84.137036715794494</v>
       </c>
     </row>
-    <row r="371" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A371" s="1" t="s">
         <v>1804</v>
       </c>
@@ -40747,7 +40792,7 @@
         <v>-81.365901920686596</v>
       </c>
     </row>
-    <row r="372" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A372" s="1" t="s">
         <v>1805</v>
       </c>
@@ -40768,6 +40813,9 @@
       </c>
       <c r="K372" s="1" t="s">
         <v>113</v>
+      </c>
+      <c r="M372" t="s">
+        <v>1810</v>
       </c>
       <c r="Q372" s="1">
         <v>166737717</v>
@@ -40813,24 +40861,24 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1723</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -40841,22 +40889,62 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-04-09T11:44:41+00:00</Document_x0020_Creation_x0020_Date>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <SharedWithUsers xmlns="8b03727f-4454-4722-b3e6-018d8dcaf2fd">
+      <UserInfo>
+        <DisplayName>Elovitz, Michael</DisplayName>
+        <AccountId>18</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ORD National Reservoir Methane Survey Members</DisplayName>
+        <AccountId>8</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001AF5FC5DD832BE4DBA6B24560DD3ADC0" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9110ddba8137efcfc9b628571238300">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="8b03727f-4454-4722-b3e6-018d8dcaf2fd" xmlns:ns6="ed970698-2d60-4bab-a048-d9be527522d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bebf8e6f5f0ff6ff908ec6e1ee4006f7" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001AF5FC5DD832BE4DBA6B24560DD3ADC0" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d40b3e6283001fb57e5088f84fb23d5e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="8b03727f-4454-4722-b3e6-018d8dcaf2fd" xmlns:ns6="ed970698-2d60-4bab-a048-d9be527522d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aadbb8160917885bdc8cfb32badaafe9" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint.v3"/>
@@ -40901,6 +40989,7 @@
                 <xsd:element ref="ns6:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns6:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns6:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns6:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -41219,6 +41308,11 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="44" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
     <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
@@ -41319,100 +41413,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-04-09T11:44:41+00:00</Document_x0020_Creation_x0020_Date>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <SharedWithUsers xmlns="8b03727f-4454-4722-b3e6-018d8dcaf2fd">
-      <UserInfo>
-        <DisplayName>Elovitz, Michael</DisplayName>
-        <AccountId>18</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ORD National Reservoir Methane Survey Members</DisplayName>
-        <AccountId>8</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8982B251-D720-483E-9E62-65A5BBA48D48}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79115C17-29BC-4C1B-9C0C-A8F448900EEC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0650EFF6-6641-4724-8CD4-C12C79553756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="8b03727f-4454-4722-b3e6-018d8dcaf2fd"/>
-    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDC4C5C1-E17F-4DA8-926C-A81F0E18ADAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -41431,4 +41446,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01D69FDD-0566-4977-AAFA-F16FE4FC4641}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79115C17-29BC-4C1B-9C0C-A8F448900EEC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8982B251-D720-483E-9E62-65A5BBA48D48}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>